<commit_message>
finished D3 except for residual analysis
</commit_message>
<xml_diff>
--- a/data_source.xlsx
+++ b/data_source.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shiyunqin/Desktop/Homework/graduate/MSCI609/homework/project/MSCI609-Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiankai/Documents/UWaterloo/MSCI609/MSCI609-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2235DA36-A617-BB43-B989-583F1C6A60A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D52DD0F9-52C6-8949-A668-636DD59D401D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="1240" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="0" windowWidth="27720" windowHeight="18000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="regression" sheetId="3" r:id="rId1"/>
@@ -24,9 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -421,7 +419,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -619,6 +617,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -800,7 +804,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -819,6 +823,8 @@
     <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2156,7 +2162,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
+    <sheetView zoomScale="84" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
     </sheetView>
@@ -4029,21 +4035,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:W52"/>
+  <dimension ref="A1:U52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+    <sheetView tabSelected="1" topLeftCell="I2" zoomScale="144" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7:U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="20" max="20" width="16" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.83203125" customWidth="1"/>
+    <col min="21" max="21" width="5.5" customWidth="1"/>
     <col min="22" max="22" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="5.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="22" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -4053,7 +4059,7 @@
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
     </row>
-    <row r="2" spans="1:23" ht="22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -4086,7 +4092,7 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:23" ht="22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="22" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>94.76</v>
       </c>
@@ -4132,7 +4138,7 @@
         <v>196.69817636363729</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="22" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>101.86</v>
       </c>
@@ -4172,23 +4178,8 @@
       <c r="M4" s="2"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
-      <c r="S4" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="T4" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="U4" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="V4" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="W4" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" ht="22" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:21" ht="22" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>103.66</v>
       </c>
@@ -4231,24 +4222,8 @@
         <f>L5*L5</f>
         <v>5170.2229090909013</v>
       </c>
-      <c r="S5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="T5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="U5" s="6">
-        <v>-1.3956077629833812</v>
-      </c>
-      <c r="V5" s="5">
-        <f>$N$12</f>
-        <v>2.0859999999999999</v>
-      </c>
-      <c r="W5" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" ht="22" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:21" ht="22" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>104.2</v>
       </c>
@@ -4276,24 +4251,8 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
-      <c r="S6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="T6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="U6" s="6">
-        <v>2.4817759855432326</v>
-      </c>
-      <c r="V6" s="5">
-        <f t="shared" ref="V6:V10" si="4">$N$12</f>
-        <v>2.0859999999999999</v>
-      </c>
-      <c r="W6" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" ht="22" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:21" ht="22" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>108.84</v>
       </c>
@@ -4319,7 +4278,7 @@
       <c r="H7" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="12">
         <f>MAX(F3:F13)</f>
         <v>0.18734219529275475</v>
       </c>
@@ -4330,24 +4289,23 @@
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
+      <c r="Q7" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="R7" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="S7" s="5" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="T7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="U7" s="6">
-        <v>-4.4490667112750275</v>
-      </c>
-      <c r="V7" s="5">
-        <f t="shared" si="4"/>
-        <v>2.0859999999999999</v>
-      </c>
-      <c r="W7" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" ht="22" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="U7" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="22" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>109.16</v>
       </c>
@@ -4380,24 +4338,24 @@
         <v>2683.4605427272695</v>
       </c>
       <c r="O8" s="4"/>
-      <c r="S8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="T8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="U8" s="6">
-        <v>-2.1962361131509156</v>
-      </c>
-      <c r="V8" s="5">
-        <f t="shared" si="4"/>
-        <v>2.0859999999999999</v>
-      </c>
-      <c r="W8" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" ht="22" x14ac:dyDescent="0.3">
+      <c r="Q8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="R8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="S8" s="6">
+        <v>1.3956077629833801</v>
+      </c>
+      <c r="T8" s="5">
+        <f>$N$12</f>
+        <v>1.7250000000000001</v>
+      </c>
+      <c r="U8" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="22" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>113.06</v>
       </c>
@@ -4430,24 +4388,24 @@
         <v>22.088501915238698</v>
       </c>
       <c r="O9" s="4"/>
-      <c r="S9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="T9" s="5" t="s">
+      <c r="Q9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="U9" s="6">
-        <v>-3.0708883735589243</v>
-      </c>
-      <c r="V9" s="5">
-        <f t="shared" si="4"/>
-        <v>2.0859999999999999</v>
-      </c>
-      <c r="W9" s="5">
+      <c r="R9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="S9" s="6">
+        <v>2.4817759855432326</v>
+      </c>
+      <c r="T9" s="5">
+        <f t="shared" ref="T6:V13" si="4">$N$12</f>
+        <v>1.7250000000000001</v>
+      </c>
+      <c r="U9" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" ht="22" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>119.21</v>
       </c>
@@ -4480,24 +4438,24 @@
         <v>-3.9297697782230632</v>
       </c>
       <c r="O10" s="4"/>
-      <c r="S10" s="5" t="s">
+      <c r="Q10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="T10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="U10" s="6">
-        <v>-3.9297697782230632</v>
-      </c>
-      <c r="V10" s="5">
+      <c r="R10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="S10" s="6">
+        <v>2.19623611315092</v>
+      </c>
+      <c r="T10" s="5">
         <f t="shared" si="4"/>
-        <v>2.0859999999999999</v>
-      </c>
-      <c r="W10" s="5">
+        <v>1.7250000000000001</v>
+      </c>
+      <c r="U10" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" ht="22" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>125.16</v>
       </c>
@@ -4525,8 +4483,24 @@
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
-    </row>
-    <row r="12" spans="1:23" ht="22" x14ac:dyDescent="0.3">
+      <c r="Q11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="R11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="S11" s="6">
+        <v>3.0708883735589199</v>
+      </c>
+      <c r="T11" s="5">
+        <f t="shared" si="4"/>
+        <v>1.7250000000000001</v>
+      </c>
+      <c r="U11" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="22" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>134.16999999999999</v>
       </c>
@@ -4555,11 +4529,27 @@
       <c r="L12" s="11"/>
       <c r="M12" s="11"/>
       <c r="N12" s="4">
-        <v>2.0859999999999999</v>
+        <v>1.7250000000000001</v>
       </c>
       <c r="O12" s="4"/>
-    </row>
-    <row r="13" spans="1:23" ht="22" x14ac:dyDescent="0.3">
+      <c r="Q12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="R12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="S12" s="6">
+        <v>3.9297697782230601</v>
+      </c>
+      <c r="T12" s="5">
+        <f t="shared" si="4"/>
+        <v>1.7250000000000001</v>
+      </c>
+      <c r="U12" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="22" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>139.24</v>
       </c>
@@ -4587,20 +4577,36 @@
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
-    </row>
-    <row r="14" spans="1:23" ht="22" x14ac:dyDescent="0.3">
+      <c r="Q13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="R13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="S13" s="6">
+        <v>4.4490667112750302</v>
+      </c>
+      <c r="T13" s="5">
+        <f t="shared" si="4"/>
+        <v>1.7250000000000001</v>
+      </c>
+      <c r="U13" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="22" x14ac:dyDescent="0.3">
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="I15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>89.42</v>
       </c>
@@ -4743,7 +4749,7 @@
       <c r="H20" t="s">
         <v>31</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="13">
         <f>MAX(F16:F26)</f>
         <v>0.12239347173510506</v>
       </c>
@@ -5039,7 +5045,7 @@
       <c r="H33" t="s">
         <v>31</v>
       </c>
-      <c r="I33">
+      <c r="I33" s="13">
         <f>MAX(F29:F39)</f>
         <v>0.13376346062836647</v>
       </c>
@@ -5335,7 +5341,7 @@
       <c r="H46" t="s">
         <v>31</v>
       </c>
-      <c r="I46">
+      <c r="I46" s="13">
         <f>MAX(F42:F52)</f>
         <v>0.1535910820571999</v>
       </c>
@@ -5485,8 +5491,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="S5:W10">
-    <sortCondition descending="1" ref="S5:S10"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="Q8:U13">
+    <sortCondition descending="1" ref="Q8:Q13"/>
   </sortState>
   <mergeCells count="4">
     <mergeCell ref="K8:M8"/>
@@ -5496,5 +5502,6 @@
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>